<commit_message>
Finished displaying app's posts dynamically
</commit_message>
<xml_diff>
--- a/TP2_Data.xlsx
+++ b/TP2_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael\OneDrive - CEGEP de Saint-JEROME\Bureau\3C4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Informatique\Session 3\Programmation d'interfaces graphiques\TPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="281" documentId="8_{1D6620D1-4BE2-44A3-AA0F-047C3EA2613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1D9112C-4013-44E9-B1A0-EE309142A93F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C27F1F-ADA9-42B6-BB5D-7496DE3CD47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28290" yWindow="975" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="1" xr2:uid="{67FAE624-DE18-42CD-98DF-9110CA9E8B51}"/>
+    <workbookView xWindow="38280" yWindow="5325" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="1" xr2:uid="{67FAE624-DE18-42CD-98DF-9110CA9E8B51}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -723,9 +723,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -737,7 +737,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -749,7 +749,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -761,7 +761,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -773,7 +773,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -796,12 +796,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -809,7 +809,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -817,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -825,7 +825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -833,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -852,10 +852,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
@@ -864,7 +864,7 @@
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -896,7 +896,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -916,7 +916,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -939,7 +939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -962,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -988,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1133,9 +1133,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1441,6 +1441,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA9D329640E8D444BB7798FD6E1353AD" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="906cb23cd56a65dfa065c3b406a06c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="347e5c82-cb7d-4657-99a2-15f9ad17bc7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7745e2992cbd53ad03f7506dd16ac53" ns2:_="">
     <xsd:import namespace="347e5c82-cb7d-4657-99a2-15f9ad17bc7a"/>
@@ -1598,29 +1613,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4586D520-BE09-4882-B3B1-406C301A854B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98D5E98A-73FB-4F58-8A75-1EE8DF6F9646}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483AF578-D750-4A89-97B9-554AD3A48306}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483AF578-D750-4A89-97B9-554AD3A48306}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98D5E98A-73FB-4F58-8A75-1EE8DF6F9646}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4586D520-BE09-4882-B3B1-406C301A854B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="347e5c82-cb7d-4657-99a2-15f9ad17bc7a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>